<commit_message>
edited the word lists. Disposed of the dictionary objects at the when each is called
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/GILD/GILDBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/GILD/GILDBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -569,6 +569,47 @@
         <v>43</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42587.819548611114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>8756</v>
+      </c>
+      <c r="D5">
+        <v>14869</v>
+      </c>
+      <c r="E5">
+        <v>1761</v>
+      </c>
+      <c r="F5">
+        <v>235</v>
+      </c>
+      <c r="G5">
+        <v>103</v>
+      </c>
+      <c r="H5">
+        <v>68</v>
+      </c>
+      <c r="I5">
+        <v>29</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>58</v>
+      </c>
+      <c r="M5">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created the htmlhelper class that removes replicated code in the googlemethods and mining classes. This will also protect against hanging from a slow internet connection
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/GILD/GILDBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/GILD/GILDBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1143,6 +1143,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42601.898865740739</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>8666</v>
+      </c>
+      <c r="D19">
+        <v>13447</v>
+      </c>
+      <c r="E19">
+        <v>1638</v>
+      </c>
+      <c r="F19">
+        <v>180</v>
+      </c>
+      <c r="G19">
+        <v>87</v>
+      </c>
+      <c r="H19">
+        <v>66</v>
+      </c>
+      <c r="I19">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>100</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the bug where the wrong positive phrase percentage was stored in the excel sheet
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/GILD/GILDBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/GILD/GILDBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:N8"/>
@@ -1158,6 +1158,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42624.619722222225</v>
+      </c>
+      <c r="B18">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>53</v>
+      </c>
+      <c r="D18">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>53</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>5964</v>
+      </c>
+      <c r="H18">
+        <v>8713</v>
+      </c>
+      <c r="I18">
+        <v>1072</v>
+      </c>
+      <c r="J18">
+        <v>116</v>
+      </c>
+      <c r="K18">
+        <v>99</v>
+      </c>
+      <c r="L18">
+        <v>31</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>